<commit_message>
annotated some, train result was showing need more data and more complex model
</commit_message>
<xml_diff>
--- a/datasets/PlateNumberPreparation/data.xlsx
+++ b/datasets/PlateNumberPreparation/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\edu\LicensePlateDetector\datasets\PlateNumberPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48913C72-31F2-4ADC-889F-95F1F604CD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACC91DF-D439-4F73-B58C-B76B5E498530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="1908" windowWidth="11532" windowHeight="8760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9732" yWindow="1224" windowWidth="11532" windowHeight="8760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12811" uniqueCount="3590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12810" uniqueCount="3603">
   <si>
     <t>image_path</t>
   </si>
@@ -10790,6 +10790,45 @@
   </si>
   <si>
     <t>MH14DX9937</t>
+  </si>
+  <si>
+    <t>30461C</t>
+  </si>
+  <si>
+    <t>YWORRY</t>
+  </si>
+  <si>
+    <t>77-ZFK-8</t>
+  </si>
+  <si>
+    <t>WOBNP300</t>
+  </si>
+  <si>
+    <t>CL31VLGP</t>
+  </si>
+  <si>
+    <t>MH15-TC-554</t>
+  </si>
+  <si>
+    <t>NP-826-D</t>
+  </si>
+  <si>
+    <t>4SH6405</t>
+  </si>
+  <si>
+    <t>7-XFT-96</t>
+  </si>
+  <si>
+    <t>TS08FM8888</t>
+  </si>
+  <si>
+    <t>MK20TC189B</t>
+  </si>
+  <si>
+    <t>KA51AA3459</t>
+  </si>
+  <si>
+    <t>DL-10NTC-0169</t>
   </si>
 </sst>
 </file>
@@ -11155,12 +11194,12 @@
   <dimension ref="A1:H2156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="57.88671875" customWidth="1"/>
+    <col min="2" max="2" width="63.33203125" customWidth="1"/>
     <col min="8" max="8" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11551,7 +11590,7 @@
         <v>3425</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -22182,7 +22221,7 @@
         <v>104</v>
       </c>
       <c r="H424" t="s">
-        <v>13</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="425" spans="1:8" x14ac:dyDescent="0.3">
@@ -22234,7 +22273,7 @@
         <v>190</v>
       </c>
       <c r="H426" t="s">
-        <v>13</v>
+        <v>3590</v>
       </c>
     </row>
     <row r="427" spans="1:8" x14ac:dyDescent="0.3">
@@ -22364,7 +22403,7 @@
         <v>18</v>
       </c>
       <c r="H431" t="s">
-        <v>13</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="432" spans="1:8" x14ac:dyDescent="0.3">
@@ -22390,7 +22429,7 @@
         <v>86</v>
       </c>
       <c r="H432" t="s">
-        <v>13</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="433" spans="1:8" x14ac:dyDescent="0.3">
@@ -22416,7 +22455,7 @@
         <v>434</v>
       </c>
       <c r="H433" t="s">
-        <v>13</v>
+        <v>3591</v>
       </c>
     </row>
     <row r="434" spans="1:8" x14ac:dyDescent="0.3">
@@ -22441,8 +22480,8 @@
       <c r="G434" t="s">
         <v>222</v>
       </c>
-      <c r="H434" t="s">
-        <v>13</v>
+      <c r="H434">
+        <v>2662</v>
       </c>
     </row>
     <row r="435" spans="1:8" x14ac:dyDescent="0.3">
@@ -22468,7 +22507,7 @@
         <v>825</v>
       </c>
       <c r="H435" t="s">
-        <v>13</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="436" spans="1:8" x14ac:dyDescent="0.3">
@@ -22520,7 +22559,7 @@
         <v>421</v>
       </c>
       <c r="H437" t="s">
-        <v>13</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="438" spans="1:8" x14ac:dyDescent="0.3">
@@ -22546,7 +22585,7 @@
         <v>417</v>
       </c>
       <c r="H438" t="s">
-        <v>13</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="439" spans="1:8" x14ac:dyDescent="0.3">
@@ -22572,7 +22611,7 @@
         <v>834</v>
       </c>
       <c r="H439" t="s">
-        <v>13</v>
+        <v>3594</v>
       </c>
     </row>
     <row r="440" spans="1:8" x14ac:dyDescent="0.3">
@@ -22624,7 +22663,7 @@
         <v>44</v>
       </c>
       <c r="H441" t="s">
-        <v>13</v>
+        <v>3595</v>
       </c>
     </row>
     <row r="442" spans="1:8" x14ac:dyDescent="0.3">
@@ -22650,7 +22689,7 @@
         <v>395</v>
       </c>
       <c r="H442" t="s">
-        <v>13</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="443" spans="1:8" x14ac:dyDescent="0.3">
@@ -22702,7 +22741,7 @@
         <v>142</v>
       </c>
       <c r="H444" t="s">
-        <v>13</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="445" spans="1:8" x14ac:dyDescent="0.3">
@@ -22754,7 +22793,7 @@
         <v>206</v>
       </c>
       <c r="H446" t="s">
-        <v>13</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="447" spans="1:8" x14ac:dyDescent="0.3">
@@ -22780,7 +22819,7 @@
         <v>615</v>
       </c>
       <c r="H447" t="s">
-        <v>13</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="448" spans="1:8" x14ac:dyDescent="0.3">
@@ -22806,7 +22845,7 @@
         <v>847</v>
       </c>
       <c r="H448" t="s">
-        <v>13</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="449" spans="1:8" x14ac:dyDescent="0.3">
@@ -22832,7 +22871,7 @@
         <v>395</v>
       </c>
       <c r="H449" t="s">
-        <v>13</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="450" spans="1:8" x14ac:dyDescent="0.3">
@@ -22884,7 +22923,7 @@
         <v>108</v>
       </c>
       <c r="H451" t="s">
-        <v>13</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="452" spans="1:8" x14ac:dyDescent="0.3">
@@ -22910,7 +22949,7 @@
         <v>68</v>
       </c>
       <c r="H452" t="s">
-        <v>13</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="453" spans="1:8" x14ac:dyDescent="0.3">
@@ -22936,7 +22975,7 @@
         <v>32</v>
       </c>
       <c r="H453" t="s">
-        <v>13</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="454" spans="1:8" x14ac:dyDescent="0.3">
@@ -22962,7 +23001,7 @@
         <v>860</v>
       </c>
       <c r="H454" t="s">
-        <v>13</v>
+        <v>3597</v>
       </c>
     </row>
     <row r="455" spans="1:8" x14ac:dyDescent="0.3">
@@ -22988,7 +23027,7 @@
         <v>467</v>
       </c>
       <c r="H455" t="s">
-        <v>13</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="456" spans="1:8" x14ac:dyDescent="0.3">
@@ -23014,7 +23053,7 @@
         <v>867</v>
       </c>
       <c r="H456" t="s">
-        <v>13</v>
+        <v>3598</v>
       </c>
     </row>
     <row r="457" spans="1:8" x14ac:dyDescent="0.3">
@@ -23066,7 +23105,7 @@
         <v>678</v>
       </c>
       <c r="H458" t="s">
-        <v>13</v>
+        <v>3599</v>
       </c>
     </row>
     <row r="459" spans="1:8" x14ac:dyDescent="0.3">
@@ -23118,7 +23157,7 @@
         <v>81</v>
       </c>
       <c r="H460" t="s">
-        <v>13</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="461" spans="1:8" x14ac:dyDescent="0.3">
@@ -23144,7 +23183,7 @@
         <v>477</v>
       </c>
       <c r="H461" t="s">
-        <v>13</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="462" spans="1:8" x14ac:dyDescent="0.3">
@@ -23170,7 +23209,7 @@
         <v>284</v>
       </c>
       <c r="H462" t="s">
-        <v>13</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="463" spans="1:8" x14ac:dyDescent="0.3">
@@ -23196,7 +23235,7 @@
         <v>166</v>
       </c>
       <c r="H463" t="s">
-        <v>13</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="464" spans="1:8" x14ac:dyDescent="0.3">
@@ -23222,7 +23261,7 @@
         <v>222</v>
       </c>
       <c r="H464" t="s">
-        <v>13</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="465" spans="1:8" x14ac:dyDescent="0.3">
@@ -23248,7 +23287,7 @@
         <v>847</v>
       </c>
       <c r="H465" t="s">
-        <v>13</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="466" spans="1:8" x14ac:dyDescent="0.3">
@@ -23274,7 +23313,7 @@
         <v>157</v>
       </c>
       <c r="H466" t="s">
-        <v>13</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="467" spans="1:8" x14ac:dyDescent="0.3">
@@ -23300,7 +23339,7 @@
         <v>219</v>
       </c>
       <c r="H467" t="s">
-        <v>13</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="468" spans="1:8" x14ac:dyDescent="0.3">
@@ -23352,7 +23391,7 @@
         <v>893</v>
       </c>
       <c r="H469" t="s">
-        <v>13</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="470" spans="1:8" x14ac:dyDescent="0.3">
@@ -23430,7 +23469,7 @@
         <v>886</v>
       </c>
       <c r="H472" t="s">
-        <v>13</v>
+        <v>3602</v>
       </c>
     </row>
     <row r="473" spans="1:8" x14ac:dyDescent="0.3">
@@ -23456,7 +23495,7 @@
         <v>93</v>
       </c>
       <c r="H473" t="s">
-        <v>13</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="474" spans="1:8" x14ac:dyDescent="0.3">
@@ -23482,7 +23521,7 @@
         <v>275</v>
       </c>
       <c r="H474" t="s">
-        <v>13</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="475" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>